<commit_message>
Game physics almost done.
</commit_message>
<xml_diff>
--- a/ref/Piece References.xlsx
+++ b/ref/Piece References.xlsx
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -380,6 +380,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -685,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="Q2:BJ69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="BA15" sqref="BA15"/>
+    <sheetView tabSelected="1" topLeftCell="R43" workbookViewId="0">
+      <selection activeCell="AX60" sqref="AX60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,7 +1748,7 @@
       <c r="AJ48" s="19"/>
       <c r="AK48" s="18"/>
     </row>
-    <row r="49" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="17:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q49" s="32"/>
       <c r="S49" s="23"/>
       <c r="T49" s="25"/>
@@ -1767,8 +1770,8 @@
       <c r="AJ49" s="25"/>
       <c r="AK49" s="26"/>
     </row>
-    <row r="50" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="17:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="17:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="17:57" x14ac:dyDescent="0.25">
       <c r="Q51" s="30" t="s">
         <v>4</v>
       </c>
@@ -1791,8 +1794,27 @@
       <c r="AI51" s="8"/>
       <c r="AJ51" s="4"/>
       <c r="AK51" s="9"/>
-    </row>
-    <row r="52" spans="17:37" x14ac:dyDescent="0.25">
+      <c r="AM51" s="36"/>
+      <c r="AN51" s="8"/>
+      <c r="AO51" s="8"/>
+      <c r="AP51" s="6"/>
+      <c r="AQ51" s="19"/>
+      <c r="AR51" s="7"/>
+      <c r="AS51" s="4"/>
+      <c r="AT51" s="4"/>
+      <c r="AU51" s="9"/>
+      <c r="AV51" s="19"/>
+      <c r="AW51" s="36"/>
+      <c r="AX51" s="4"/>
+      <c r="AY51" s="8"/>
+      <c r="AZ51" s="9"/>
+      <c r="BA51" s="10"/>
+      <c r="BB51" s="7"/>
+      <c r="BC51" s="8"/>
+      <c r="BD51" s="4"/>
+      <c r="BE51" s="9"/>
+    </row>
+    <row r="52" spans="17:57" x14ac:dyDescent="0.25">
       <c r="Q52" s="31"/>
       <c r="S52" s="15"/>
       <c r="T52" s="12"/>
@@ -1813,8 +1835,27 @@
       <c r="AI52" s="12"/>
       <c r="AJ52" s="12"/>
       <c r="AK52" s="18"/>
-    </row>
-    <row r="53" spans="17:37" x14ac:dyDescent="0.25">
+      <c r="AM52" s="17"/>
+      <c r="AN52" s="12"/>
+      <c r="AO52" s="19"/>
+      <c r="AP52" s="14"/>
+      <c r="AQ52" s="19"/>
+      <c r="AR52" s="17"/>
+      <c r="AS52" s="12"/>
+      <c r="AT52" s="19"/>
+      <c r="AU52" s="14"/>
+      <c r="AV52" s="19"/>
+      <c r="AW52" s="15"/>
+      <c r="AX52" s="12"/>
+      <c r="AY52" s="12"/>
+      <c r="AZ52" s="18"/>
+      <c r="BA52" s="10"/>
+      <c r="BB52" s="15"/>
+      <c r="BC52" s="12"/>
+      <c r="BD52" s="12"/>
+      <c r="BE52" s="18"/>
+    </row>
+    <row r="53" spans="17:57" x14ac:dyDescent="0.25">
       <c r="Q53" s="31"/>
       <c r="S53" s="15"/>
       <c r="T53" s="19"/>
@@ -1835,8 +1876,27 @@
       <c r="AI53" s="12"/>
       <c r="AJ53" s="19"/>
       <c r="AK53" s="18"/>
-    </row>
-    <row r="54" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM53" s="15"/>
+      <c r="AN53" s="12"/>
+      <c r="AO53" s="12"/>
+      <c r="AP53" s="14"/>
+      <c r="AQ53" s="19"/>
+      <c r="AR53" s="17"/>
+      <c r="AS53" s="19"/>
+      <c r="AT53" s="19"/>
+      <c r="AU53" s="14"/>
+      <c r="AV53" s="19"/>
+      <c r="AW53" s="15"/>
+      <c r="AX53" s="19"/>
+      <c r="AY53" s="12"/>
+      <c r="AZ53" s="18"/>
+      <c r="BA53" s="10"/>
+      <c r="BB53" s="17"/>
+      <c r="BC53" s="12"/>
+      <c r="BD53" s="19"/>
+      <c r="BE53" s="18"/>
+    </row>
+    <row r="54" spans="17:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q54" s="32"/>
       <c r="S54" s="23"/>
       <c r="T54" s="25"/>
@@ -1857,9 +1917,28 @@
       <c r="AI54" s="25"/>
       <c r="AJ54" s="25"/>
       <c r="AK54" s="26"/>
-    </row>
-    <row r="55" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="17:37" x14ac:dyDescent="0.25">
+      <c r="AM54" s="23"/>
+      <c r="AN54" s="25"/>
+      <c r="AO54" s="25"/>
+      <c r="AP54" s="26"/>
+      <c r="AQ54" s="19"/>
+      <c r="AR54" s="23"/>
+      <c r="AS54" s="21"/>
+      <c r="AT54" s="21"/>
+      <c r="AU54" s="22"/>
+      <c r="AV54" s="19"/>
+      <c r="AW54" s="20"/>
+      <c r="AX54" s="21"/>
+      <c r="AY54" s="21"/>
+      <c r="AZ54" s="26"/>
+      <c r="BA54" s="10"/>
+      <c r="BB54" s="23"/>
+      <c r="BC54" s="25"/>
+      <c r="BD54" s="25"/>
+      <c r="BE54" s="26"/>
+    </row>
+    <row r="55" spans="17:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="17:57" x14ac:dyDescent="0.25">
       <c r="Q56" s="30" t="s">
         <v>5</v>
       </c>
@@ -1881,7 +1960,7 @@
       <c r="AJ56" s="8"/>
       <c r="AK56" s="9"/>
     </row>
-    <row r="57" spans="17:37" x14ac:dyDescent="0.25">
+    <row r="57" spans="17:57" x14ac:dyDescent="0.25">
       <c r="Q57" s="31"/>
       <c r="S57" s="15"/>
       <c r="T57" s="19"/>
@@ -1901,7 +1980,7 @@
       <c r="AJ57" s="12"/>
       <c r="AK57" s="18"/>
     </row>
-    <row r="58" spans="17:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="17:57" x14ac:dyDescent="0.25">
       <c r="Q58" s="31"/>
       <c r="S58" s="17"/>
       <c r="T58" s="12"/>
@@ -1921,7 +2000,7 @@
       <c r="AJ58" s="12"/>
       <c r="AK58" s="18"/>
     </row>
-    <row r="59" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="17:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q59" s="31"/>
       <c r="S59" s="23"/>
       <c r="T59" s="25"/>
@@ -1941,7 +2020,7 @@
       <c r="AJ59" s="24"/>
       <c r="AK59" s="26"/>
     </row>
-    <row r="60" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="17:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q60" s="31"/>
       <c r="X60" s="10"/>
       <c r="Y60" s="10"/>
@@ -1958,7 +2037,7 @@
       <c r="AJ60" s="10"/>
       <c r="AK60" s="10"/>
     </row>
-    <row r="61" spans="17:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="17:57" x14ac:dyDescent="0.25">
       <c r="Q61" s="31"/>
       <c r="S61" s="7"/>
       <c r="T61" s="8"/>
@@ -1979,7 +2058,7 @@
       <c r="AJ61" s="4"/>
       <c r="AK61" s="9"/>
     </row>
-    <row r="62" spans="17:37" x14ac:dyDescent="0.25">
+    <row r="62" spans="17:57" x14ac:dyDescent="0.25">
       <c r="Q62" s="31"/>
       <c r="S62" s="17"/>
       <c r="T62" s="12"/>
@@ -2000,7 +2079,7 @@
       <c r="AJ62" s="12"/>
       <c r="AK62" s="18"/>
     </row>
-    <row r="63" spans="17:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="17:57" x14ac:dyDescent="0.25">
       <c r="Q63" s="31"/>
       <c r="S63" s="15"/>
       <c r="T63" s="19"/>
@@ -2021,7 +2100,7 @@
       <c r="AJ63" s="19"/>
       <c r="AK63" s="18"/>
     </row>
-    <row r="64" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="17:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q64" s="32"/>
       <c r="S64" s="23"/>
       <c r="T64" s="25"/>
@@ -2127,11 +2206,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="X4:AA4"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="AH4:AK4"/>
-    <mergeCell ref="Q51:Q54"/>
+    <mergeCell ref="AR2:BJ2"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="AH2:AK2"/>
     <mergeCell ref="Q56:Q64"/>
     <mergeCell ref="Q66:Q69"/>
     <mergeCell ref="Q36:Q44"/>
@@ -2141,11 +2220,11 @@
     <mergeCell ref="Q21:Q24"/>
     <mergeCell ref="Q26:Q29"/>
     <mergeCell ref="Q31:Q34"/>
-    <mergeCell ref="AR2:BJ2"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="X4:AA4"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="AH4:AK4"/>
+    <mergeCell ref="Q51:Q54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Level editor and play scene
</commit_message>
<xml_diff>
--- a/ref/Piece References.xlsx
+++ b/ref/Piece References.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>V</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -278,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -370,6 +376,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -377,18 +398,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -692,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="Q2:BJ79"/>
+  <dimension ref="Q2:BJ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41:Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,78 +716,78 @@
   </cols>
   <sheetData>
     <row r="2" spans="17:62" x14ac:dyDescent="0.25">
-      <c r="S2" s="34">
+      <c r="S2" s="32">
         <v>0</v>
       </c>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="X2" s="34">
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="X2" s="32">
         <v>1</v>
       </c>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AC2" s="34">
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AC2" s="32">
         <v>2</v>
       </c>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AH2" s="34">
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AH2" s="32">
         <v>3</v>
       </c>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AR2" s="31" t="s">
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AR2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
-      <c r="AW2" s="32"/>
-      <c r="AX2" s="32"/>
-      <c r="AY2" s="32"/>
-      <c r="AZ2" s="32"/>
-      <c r="BA2" s="32"/>
-      <c r="BB2" s="32"/>
-      <c r="BC2" s="32"/>
-      <c r="BD2" s="32"/>
-      <c r="BE2" s="32"/>
-      <c r="BF2" s="32"/>
-      <c r="BG2" s="32"/>
-      <c r="BH2" s="32"/>
-      <c r="BI2" s="32"/>
-      <c r="BJ2" s="33"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="37"/>
+      <c r="AX2" s="37"/>
+      <c r="AY2" s="37"/>
+      <c r="AZ2" s="37"/>
+      <c r="BA2" s="37"/>
+      <c r="BB2" s="37"/>
+      <c r="BC2" s="37"/>
+      <c r="BD2" s="37"/>
+      <c r="BE2" s="37"/>
+      <c r="BF2" s="37"/>
+      <c r="BG2" s="37"/>
+      <c r="BH2" s="37"/>
+      <c r="BI2" s="37"/>
+      <c r="BJ2" s="38"/>
     </row>
     <row r="3" spans="17:62" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="17:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="S4" s="34">
+      <c r="S4" s="32">
         <v>4</v>
       </c>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="X4" s="34">
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="X4" s="32">
         <v>5</v>
       </c>
-      <c r="Y4" s="34"/>
-      <c r="Z4" s="34"/>
-      <c r="AA4" s="34"/>
-      <c r="AC4" s="34">
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="32"/>
+      <c r="AC4" s="32">
         <v>6</v>
       </c>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
-      <c r="AH4" s="34">
+      <c r="AD4" s="32"/>
+      <c r="AE4" s="32"/>
+      <c r="AF4" s="32"/>
+      <c r="AH4" s="32">
         <v>7</v>
       </c>
-      <c r="AI4" s="34"/>
-      <c r="AJ4" s="34"/>
-      <c r="AK4" s="34"/>
+      <c r="AI4" s="32"/>
+      <c r="AJ4" s="32"/>
+      <c r="AK4" s="32"/>
       <c r="AR4" s="3"/>
       <c r="AS4" s="5" t="s">
         <v>1</v>
@@ -830,7 +839,7 @@
       <c r="BJ5" s="14"/>
     </row>
     <row r="6" spans="17:62" x14ac:dyDescent="0.25">
-      <c r="Q6" s="35" t="s">
+      <c r="Q6" s="33" t="s">
         <v>7</v>
       </c>
       <c r="S6" s="7"/>
@@ -870,7 +879,7 @@
       <c r="BJ6" s="14"/>
     </row>
     <row r="7" spans="17:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q7" s="36"/>
+      <c r="Q7" s="34"/>
       <c r="S7" s="15"/>
       <c r="T7" s="12"/>
       <c r="U7" s="19"/>
@@ -910,7 +919,7 @@
       <c r="BJ7" s="22"/>
     </row>
     <row r="8" spans="17:62" x14ac:dyDescent="0.25">
-      <c r="Q8" s="36"/>
+      <c r="Q8" s="34"/>
       <c r="S8" s="15"/>
       <c r="T8" s="12"/>
       <c r="U8" s="19"/>
@@ -932,7 +941,7 @@
       <c r="AK8" s="16"/>
     </row>
     <row r="9" spans="17:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q9" s="36"/>
+      <c r="Q9" s="34"/>
       <c r="S9" s="23"/>
       <c r="T9" s="24"/>
       <c r="U9" s="24"/>
@@ -983,7 +992,7 @@
       <c r="BJ9" s="27"/>
     </row>
     <row r="10" spans="17:62" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q10" s="36"/>
+      <c r="Q10" s="34"/>
       <c r="S10" s="19"/>
       <c r="T10" s="19"/>
       <c r="U10" s="19"/>
@@ -1026,7 +1035,7 @@
       <c r="BJ10" s="27"/>
     </row>
     <row r="11" spans="17:62" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Q11" s="36"/>
+      <c r="Q11" s="34"/>
       <c r="S11" s="7"/>
       <c r="T11" s="8"/>
       <c r="U11" s="4"/>
@@ -1069,7 +1078,7 @@
       <c r="BJ11" s="27"/>
     </row>
     <row r="12" spans="17:62" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Q12" s="36"/>
+      <c r="Q12" s="34"/>
       <c r="S12" s="15"/>
       <c r="T12" s="19"/>
       <c r="U12" s="12"/>
@@ -1110,7 +1119,7 @@
       <c r="BJ12" s="27"/>
     </row>
     <row r="13" spans="17:62" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Q13" s="36"/>
+      <c r="Q13" s="34"/>
       <c r="S13" s="15"/>
       <c r="T13" s="19"/>
       <c r="U13" s="12"/>
@@ -1132,7 +1141,7 @@
       <c r="AK13" s="16"/>
     </row>
     <row r="14" spans="17:62" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q14" s="37"/>
+      <c r="Q14" s="35"/>
       <c r="S14" s="23"/>
       <c r="T14" s="24"/>
       <c r="U14" s="24"/>
@@ -1155,7 +1164,7 @@
     </row>
     <row r="15" spans="17:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="17:62" x14ac:dyDescent="0.25">
-      <c r="Q16" s="35" t="s">
+      <c r="Q16" s="33" t="s">
         <v>8</v>
       </c>
       <c r="S16" s="7"/>
@@ -1179,7 +1188,7 @@
       <c r="AK16" s="9"/>
     </row>
     <row r="17" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q17" s="36"/>
+      <c r="Q17" s="34"/>
       <c r="S17" s="15"/>
       <c r="T17" s="19"/>
       <c r="U17" s="12"/>
@@ -1201,7 +1210,7 @@
       <c r="AK17" s="18"/>
     </row>
     <row r="18" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q18" s="36"/>
+      <c r="Q18" s="34"/>
       <c r="S18" s="17"/>
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
@@ -1223,7 +1232,7 @@
       <c r="AK18" s="18"/>
     </row>
     <row r="19" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q19" s="36"/>
+      <c r="Q19" s="34"/>
       <c r="S19" s="23"/>
       <c r="T19" s="25"/>
       <c r="U19" s="25"/>
@@ -1245,10 +1254,10 @@
       <c r="AK19" s="26"/>
     </row>
     <row r="20" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q20" s="36"/>
+      <c r="Q20" s="34"/>
     </row>
     <row r="21" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q21" s="36"/>
+      <c r="Q21" s="34"/>
       <c r="R21" s="2"/>
       <c r="S21" s="7"/>
       <c r="T21" s="8"/>
@@ -1271,7 +1280,7 @@
       <c r="AK21" s="9"/>
     </row>
     <row r="22" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q22" s="36"/>
+      <c r="Q22" s="34"/>
       <c r="R22" s="2"/>
       <c r="S22" s="15"/>
       <c r="T22" s="12"/>
@@ -1294,7 +1303,7 @@
       <c r="AK22" s="18"/>
     </row>
     <row r="23" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q23" s="36"/>
+      <c r="Q23" s="34"/>
       <c r="R23" s="2"/>
       <c r="S23" s="17"/>
       <c r="T23" s="12"/>
@@ -1317,7 +1326,7 @@
       <c r="AK23" s="18"/>
     </row>
     <row r="24" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q24" s="37"/>
+      <c r="Q24" s="35"/>
       <c r="R24" s="2"/>
       <c r="S24" s="23"/>
       <c r="T24" s="25"/>
@@ -1341,7 +1350,7 @@
     </row>
     <row r="25" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q26" s="35" t="s">
+      <c r="Q26" s="33" t="s">
         <v>6</v>
       </c>
       <c r="S26" s="7"/>
@@ -1365,7 +1374,7 @@
       <c r="AK26" s="9"/>
     </row>
     <row r="27" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q27" s="36"/>
+      <c r="Q27" s="34"/>
       <c r="S27" s="15"/>
       <c r="T27" s="12"/>
       <c r="U27" s="12"/>
@@ -1387,7 +1396,7 @@
       <c r="AK27" s="18"/>
     </row>
     <row r="28" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q28" s="36"/>
+      <c r="Q28" s="34"/>
       <c r="S28" s="15"/>
       <c r="T28" s="12"/>
       <c r="U28" s="12"/>
@@ -1409,7 +1418,7 @@
       <c r="AK28" s="18"/>
     </row>
     <row r="29" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q29" s="36"/>
+      <c r="Q29" s="34"/>
       <c r="S29" s="23"/>
       <c r="T29" s="24"/>
       <c r="U29" s="25"/>
@@ -1431,7 +1440,7 @@
       <c r="AK29" s="26"/>
     </row>
     <row r="30" spans="17:37" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q30" s="36"/>
+      <c r="Q30" s="34"/>
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
       <c r="U30" s="19"/>
@@ -1453,7 +1462,7 @@
       <c r="AK30" s="19"/>
     </row>
     <row r="31" spans="17:37" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Q31" s="36"/>
+      <c r="Q31" s="34"/>
       <c r="S31" s="7"/>
       <c r="T31" s="8"/>
       <c r="U31" s="8"/>
@@ -1475,7 +1484,7 @@
       <c r="AK31" s="9"/>
     </row>
     <row r="32" spans="17:37" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Q32" s="36"/>
+      <c r="Q32" s="34"/>
       <c r="S32" s="15"/>
       <c r="T32" s="12"/>
       <c r="U32" s="12"/>
@@ -1497,7 +1506,7 @@
       <c r="AK32" s="16"/>
     </row>
     <row r="33" spans="17:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Q33" s="36"/>
+      <c r="Q33" s="34"/>
       <c r="S33" s="15"/>
       <c r="T33" s="12"/>
       <c r="U33" s="12"/>
@@ -1519,7 +1528,7 @@
       <c r="AK33" s="18"/>
     </row>
     <row r="34" spans="17:45" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q34" s="37"/>
+      <c r="Q34" s="35"/>
       <c r="S34" s="23"/>
       <c r="T34" s="25"/>
       <c r="U34" s="24"/>
@@ -1542,7 +1551,7 @@
     </row>
     <row r="35" spans="17:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="17:45" x14ac:dyDescent="0.25">
-      <c r="Q36" s="35" t="s">
+      <c r="Q36" s="33" t="s">
         <v>9</v>
       </c>
       <c r="S36" s="7"/>
@@ -1566,7 +1575,7 @@
       <c r="AK36" s="9"/>
     </row>
     <row r="37" spans="17:45" x14ac:dyDescent="0.25">
-      <c r="Q37" s="36"/>
+      <c r="Q37" s="34"/>
       <c r="S37" s="17"/>
       <c r="T37" s="19"/>
       <c r="U37" s="12"/>
@@ -1588,7 +1597,7 @@
       <c r="AK37" s="18"/>
     </row>
     <row r="38" spans="17:45" x14ac:dyDescent="0.25">
-      <c r="Q38" s="36"/>
+      <c r="Q38" s="34"/>
       <c r="S38" s="17"/>
       <c r="T38" s="12"/>
       <c r="U38" s="12"/>
@@ -1610,7 +1619,7 @@
       <c r="AK38" s="18"/>
     </row>
     <row r="39" spans="17:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q39" s="37"/>
+      <c r="Q39" s="35"/>
       <c r="S39" s="23"/>
       <c r="T39" s="25"/>
       <c r="U39" s="25"/>
@@ -1633,7 +1642,7 @@
     </row>
     <row r="40" spans="17:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="17:45" x14ac:dyDescent="0.25">
-      <c r="Q41" s="35" t="s">
+      <c r="Q41" s="33" t="s">
         <v>3</v>
       </c>
       <c r="S41" s="30"/>
@@ -1646,18 +1655,18 @@
       <c r="Z41" s="4"/>
       <c r="AA41" s="9"/>
       <c r="AB41" s="10"/>
-      <c r="AC41" s="30"/>
+      <c r="AC41" s="7"/>
       <c r="AD41" s="4"/>
-      <c r="AE41" s="8"/>
+      <c r="AE41" s="4"/>
       <c r="AF41" s="9"/>
       <c r="AG41" s="10"/>
-      <c r="AH41" s="7"/>
+      <c r="AH41" s="30"/>
       <c r="AI41" s="8"/>
-      <c r="AJ41" s="4"/>
+      <c r="AJ41" s="8"/>
       <c r="AK41" s="9"/>
     </row>
     <row r="42" spans="17:45" x14ac:dyDescent="0.25">
-      <c r="Q42" s="36"/>
+      <c r="Q42" s="34"/>
       <c r="S42" s="15"/>
       <c r="T42" s="12"/>
       <c r="U42" s="19"/>
@@ -1679,7 +1688,7 @@
       <c r="AK42" s="18"/>
     </row>
     <row r="43" spans="17:45" x14ac:dyDescent="0.25">
-      <c r="Q43" s="36"/>
+      <c r="Q43" s="34"/>
       <c r="S43" s="15"/>
       <c r="T43" s="12"/>
       <c r="U43" s="12"/>
@@ -1690,21 +1699,21 @@
       <c r="Z43" s="19"/>
       <c r="AA43" s="14"/>
       <c r="AB43" s="10"/>
-      <c r="AC43" s="15"/>
+      <c r="AC43" s="17"/>
       <c r="AD43" s="12"/>
-      <c r="AE43" s="12"/>
+      <c r="AE43" s="19"/>
       <c r="AF43" s="18"/>
       <c r="AG43" s="10"/>
-      <c r="AH43" s="17"/>
+      <c r="AH43" s="15"/>
       <c r="AI43" s="19"/>
-      <c r="AJ43" s="19"/>
+      <c r="AJ43" s="12"/>
       <c r="AK43" s="18"/>
       <c r="AS43" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="44" spans="17:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q44" s="37"/>
+      <c r="Q44" s="35"/>
       <c r="S44" s="23"/>
       <c r="T44" s="25"/>
       <c r="U44" s="25"/>
@@ -1715,9 +1724,9 @@
       <c r="Z44" s="21"/>
       <c r="AA44" s="22"/>
       <c r="AB44" s="10"/>
-      <c r="AC44" s="20"/>
-      <c r="AD44" s="21"/>
-      <c r="AE44" s="21"/>
+      <c r="AC44" s="23"/>
+      <c r="AD44" s="25"/>
+      <c r="AE44" s="25"/>
       <c r="AF44" s="26"/>
       <c r="AG44" s="10"/>
       <c r="AH44" s="23"/>
@@ -1727,7 +1736,7 @@
     </row>
     <row r="45" spans="17:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="17:45" x14ac:dyDescent="0.25">
-      <c r="Q46" s="35" t="s">
+      <c r="Q46" s="33" t="s">
         <v>10</v>
       </c>
       <c r="S46" s="7"/>
@@ -1751,7 +1760,7 @@
       <c r="AK46" s="6"/>
     </row>
     <row r="47" spans="17:45" x14ac:dyDescent="0.25">
-      <c r="Q47" s="36"/>
+      <c r="Q47" s="34"/>
       <c r="S47" s="17"/>
       <c r="T47" s="12"/>
       <c r="U47" s="19"/>
@@ -1773,7 +1782,7 @@
       <c r="AK47" s="14"/>
     </row>
     <row r="48" spans="17:45" x14ac:dyDescent="0.25">
-      <c r="Q48" s="36"/>
+      <c r="Q48" s="34"/>
       <c r="S48" s="15"/>
       <c r="T48" s="12"/>
       <c r="U48" s="19"/>
@@ -1795,7 +1804,7 @@
       <c r="AK48" s="14"/>
     </row>
     <row r="49" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q49" s="36"/>
+      <c r="Q49" s="34"/>
       <c r="S49" s="23"/>
       <c r="T49" s="21"/>
       <c r="U49" s="21"/>
@@ -1817,99 +1826,95 @@
       <c r="AK49" s="26"/>
     </row>
     <row r="50" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q50" s="36"/>
+      <c r="Q50" s="34"/>
     </row>
     <row r="51" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q51" s="36"/>
-      <c r="S51" s="7"/>
+      <c r="Q51" s="34"/>
+      <c r="S51" s="30"/>
       <c r="T51" s="4"/>
       <c r="U51" s="8"/>
-      <c r="V51" s="6"/>
+      <c r="V51" s="9"/>
       <c r="W51" s="10"/>
       <c r="X51" s="7"/>
-      <c r="Y51" s="4"/>
-      <c r="Z51" s="8"/>
+      <c r="Y51" s="8"/>
+      <c r="Z51" s="4"/>
       <c r="AA51" s="9"/>
-      <c r="AB51" s="10"/>
-      <c r="AC51" s="30"/>
+      <c r="AC51" s="7"/>
       <c r="AD51" s="4"/>
       <c r="AE51" s="8"/>
-      <c r="AF51" s="9"/>
+      <c r="AF51" s="6"/>
       <c r="AG51" s="10"/>
       <c r="AH51" s="7"/>
-      <c r="AI51" s="8"/>
-      <c r="AJ51" s="4"/>
+      <c r="AI51" s="4"/>
+      <c r="AJ51" s="8"/>
       <c r="AK51" s="9"/>
     </row>
     <row r="52" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q52" s="36"/>
-      <c r="S52" s="17"/>
+      <c r="Q52" s="34"/>
+      <c r="S52" s="15"/>
       <c r="T52" s="12"/>
-      <c r="U52" s="19"/>
-      <c r="V52" s="14"/>
+      <c r="U52" s="12"/>
+      <c r="V52" s="18"/>
       <c r="W52" s="10"/>
       <c r="X52" s="17"/>
       <c r="Y52" s="12"/>
       <c r="Z52" s="12"/>
-      <c r="AA52" s="14"/>
-      <c r="AB52" s="10"/>
-      <c r="AC52" s="15"/>
+      <c r="AA52" s="18"/>
+      <c r="AC52" s="17"/>
       <c r="AD52" s="12"/>
-      <c r="AE52" s="12"/>
-      <c r="AF52" s="18"/>
+      <c r="AE52" s="19"/>
+      <c r="AF52" s="14"/>
       <c r="AG52" s="10"/>
       <c r="AH52" s="17"/>
       <c r="AI52" s="12"/>
       <c r="AJ52" s="12"/>
-      <c r="AK52" s="18"/>
+      <c r="AK52" s="14"/>
     </row>
     <row r="53" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q53" s="36"/>
+      <c r="Q53" s="34"/>
       <c r="S53" s="15"/>
       <c r="T53" s="12"/>
-      <c r="U53" s="12"/>
-      <c r="V53" s="14"/>
+      <c r="U53" s="19"/>
+      <c r="V53" s="18"/>
       <c r="W53" s="10"/>
-      <c r="X53" s="17"/>
-      <c r="Y53" s="19"/>
+      <c r="X53" s="15"/>
+      <c r="Y53" s="12"/>
       <c r="Z53" s="19"/>
-      <c r="AA53" s="14"/>
-      <c r="AB53" s="10"/>
+      <c r="AA53" s="18"/>
       <c r="AC53" s="15"/>
       <c r="AD53" s="12"/>
-      <c r="AE53" s="19"/>
-      <c r="AF53" s="18"/>
+      <c r="AE53" s="12"/>
+      <c r="AF53" s="14"/>
       <c r="AG53" s="10"/>
-      <c r="AH53" s="15"/>
-      <c r="AI53" s="12"/>
+      <c r="AH53" s="17"/>
+      <c r="AI53" s="19"/>
       <c r="AJ53" s="19"/>
-      <c r="AK53" s="18"/>
+      <c r="AK53" s="14"/>
     </row>
     <row r="54" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q54" s="37"/>
-      <c r="S54" s="23"/>
-      <c r="T54" s="25"/>
-      <c r="U54" s="25"/>
+      <c r="Q54" s="35"/>
+      <c r="S54" s="20"/>
+      <c r="T54" s="21"/>
+      <c r="U54" s="21"/>
       <c r="V54" s="26"/>
       <c r="W54" s="10"/>
       <c r="X54" s="23"/>
-      <c r="Y54" s="21"/>
-      <c r="Z54" s="21"/>
-      <c r="AA54" s="22"/>
-      <c r="AB54" s="10"/>
-      <c r="AC54" s="20"/>
-      <c r="AD54" s="21"/>
-      <c r="AE54" s="21"/>
+      <c r="Y54" s="25"/>
+      <c r="Z54" s="25"/>
+      <c r="AA54" s="26"/>
+      <c r="AC54" s="23"/>
+      <c r="AD54" s="25"/>
+      <c r="AE54" s="25"/>
       <c r="AF54" s="26"/>
       <c r="AG54" s="10"/>
       <c r="AH54" s="23"/>
-      <c r="AI54" s="25"/>
-      <c r="AJ54" s="25"/>
-      <c r="AK54" s="26"/>
+      <c r="AI54" s="21"/>
+      <c r="AJ54" s="21"/>
+      <c r="AK54" s="22"/>
     </row>
     <row r="55" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q56" s="35" t="s">
+      <c r="Q56" s="33" t="s">
         <v>11</v>
       </c>
       <c r="S56" s="30"/>
@@ -1933,7 +1938,7 @@
       <c r="AK56" s="6"/>
     </row>
     <row r="57" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q57" s="36"/>
+      <c r="Q57" s="34"/>
       <c r="S57" s="15"/>
       <c r="T57" s="12"/>
       <c r="U57" s="19"/>
@@ -1955,7 +1960,7 @@
       <c r="AK57" s="14"/>
     </row>
     <row r="58" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q58" s="36"/>
+      <c r="Q58" s="34"/>
       <c r="S58" s="15"/>
       <c r="T58" s="12"/>
       <c r="U58" s="19"/>
@@ -1977,7 +1982,7 @@
       <c r="AK58" s="14"/>
     </row>
     <row r="59" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q59" s="37"/>
+      <c r="Q59" s="35"/>
       <c r="S59" s="23"/>
       <c r="T59" s="21"/>
       <c r="U59" s="21"/>
@@ -2000,7 +2005,7 @@
     </row>
     <row r="60" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q61" s="35" t="s">
+      <c r="Q61" s="33" t="s">
         <v>4</v>
       </c>
       <c r="S61" s="30"/>
@@ -2024,7 +2029,7 @@
       <c r="AK61" s="9"/>
     </row>
     <row r="62" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q62" s="36"/>
+      <c r="Q62" s="34"/>
       <c r="S62" s="17"/>
       <c r="T62" s="12"/>
       <c r="U62" s="19"/>
@@ -2046,7 +2051,7 @@
       <c r="AK62" s="18"/>
     </row>
     <row r="63" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q63" s="36"/>
+      <c r="Q63" s="34"/>
       <c r="S63" s="15"/>
       <c r="T63" s="12"/>
       <c r="U63" s="12"/>
@@ -2068,7 +2073,7 @@
       <c r="AK63" s="18"/>
     </row>
     <row r="64" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q64" s="37"/>
+      <c r="Q64" s="35"/>
       <c r="S64" s="23"/>
       <c r="T64" s="25"/>
       <c r="U64" s="25"/>
@@ -2091,7 +2096,7 @@
     </row>
     <row r="65" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="66" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q66" s="35" t="s">
+      <c r="Q66" s="33" t="s">
         <v>5</v>
       </c>
       <c r="S66" s="7"/>
@@ -2113,7 +2118,7 @@
       <c r="AK66" s="9"/>
     </row>
     <row r="67" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q67" s="36"/>
+      <c r="Q67" s="34"/>
       <c r="S67" s="15"/>
       <c r="T67" s="19"/>
       <c r="U67" s="12"/>
@@ -2133,7 +2138,7 @@
       <c r="AK67" s="18"/>
     </row>
     <row r="68" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q68" s="36"/>
+      <c r="Q68" s="34"/>
       <c r="S68" s="17"/>
       <c r="T68" s="12"/>
       <c r="U68" s="12"/>
@@ -2153,7 +2158,7 @@
       <c r="AK68" s="18"/>
     </row>
     <row r="69" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q69" s="36"/>
+      <c r="Q69" s="34"/>
       <c r="S69" s="23"/>
       <c r="T69" s="25"/>
       <c r="U69" s="25"/>
@@ -2173,7 +2178,7 @@
       <c r="AK69" s="26"/>
     </row>
     <row r="70" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q70" s="36"/>
+      <c r="Q70" s="34"/>
       <c r="X70" s="10"/>
       <c r="Y70" s="10"/>
       <c r="Z70" s="10"/>
@@ -2190,7 +2195,7 @@
       <c r="AK70" s="10"/>
     </row>
     <row r="71" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q71" s="36"/>
+      <c r="Q71" s="34"/>
       <c r="S71" s="7"/>
       <c r="T71" s="8"/>
       <c r="U71" s="8"/>
@@ -2211,7 +2216,7 @@
       <c r="AK71" s="9"/>
     </row>
     <row r="72" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q72" s="36"/>
+      <c r="Q72" s="34"/>
       <c r="S72" s="17"/>
       <c r="T72" s="12"/>
       <c r="U72" s="12"/>
@@ -2232,7 +2237,7 @@
       <c r="AK72" s="18"/>
     </row>
     <row r="73" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q73" s="36"/>
+      <c r="Q73" s="34"/>
       <c r="S73" s="15"/>
       <c r="T73" s="19"/>
       <c r="U73" s="12"/>
@@ -2253,7 +2258,7 @@
       <c r="AK73" s="18"/>
     </row>
     <row r="74" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q74" s="37"/>
+      <c r="Q74" s="35"/>
       <c r="S74" s="23"/>
       <c r="T74" s="25"/>
       <c r="U74" s="25"/>
@@ -2275,7 +2280,7 @@
     </row>
     <row r="75" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="76" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q76" s="35" t="s">
+      <c r="Q76" s="33" t="s">
         <v>0</v>
       </c>
       <c r="S76" s="3"/>
@@ -2297,7 +2302,7 @@
       <c r="AK76" s="9"/>
     </row>
     <row r="77" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q77" s="36"/>
+      <c r="Q77" s="34"/>
       <c r="S77" s="11"/>
       <c r="T77" s="12"/>
       <c r="U77" s="13"/>
@@ -2317,7 +2322,7 @@
       <c r="AK77" s="18"/>
     </row>
     <row r="78" spans="17:37" x14ac:dyDescent="0.25">
-      <c r="Q78" s="36"/>
+      <c r="Q78" s="34"/>
       <c r="S78" s="11"/>
       <c r="T78" s="12"/>
       <c r="U78" s="12"/>
@@ -2337,7 +2342,7 @@
       <c r="AK78" s="18"/>
     </row>
     <row r="79" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q79" s="37"/>
+      <c r="Q79" s="35"/>
       <c r="S79" s="20"/>
       <c r="T79" s="21"/>
       <c r="U79" s="21"/>
@@ -2356,8 +2361,204 @@
       <c r="AJ79" s="25"/>
       <c r="AK79" s="26"/>
     </row>
+    <row r="80" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="17:37" x14ac:dyDescent="0.25">
+      <c r="Q81" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="S81" s="7"/>
+      <c r="T81" s="8"/>
+      <c r="U81" s="8"/>
+      <c r="V81" s="9"/>
+      <c r="W81" s="10"/>
+      <c r="X81" s="7"/>
+      <c r="Y81" s="8"/>
+      <c r="Z81" s="8"/>
+      <c r="AA81" s="9"/>
+      <c r="AB81" s="10"/>
+      <c r="AC81" s="7"/>
+      <c r="AD81" s="8"/>
+      <c r="AE81" s="8"/>
+      <c r="AF81" s="9"/>
+      <c r="AG81" s="10"/>
+      <c r="AH81" s="7"/>
+      <c r="AI81" s="8"/>
+      <c r="AJ81" s="8"/>
+      <c r="AK81" s="9"/>
+    </row>
+    <row r="82" spans="17:37" x14ac:dyDescent="0.25">
+      <c r="Q82" s="34"/>
+      <c r="S82" s="15"/>
+      <c r="T82" s="19"/>
+      <c r="U82" s="19"/>
+      <c r="V82" s="18"/>
+      <c r="W82" s="10"/>
+      <c r="X82" s="15"/>
+      <c r="Y82" s="19"/>
+      <c r="Z82" s="19"/>
+      <c r="AA82" s="18"/>
+      <c r="AB82" s="10"/>
+      <c r="AC82" s="15"/>
+      <c r="AD82" s="19"/>
+      <c r="AE82" s="19"/>
+      <c r="AF82" s="18"/>
+      <c r="AG82" s="10"/>
+      <c r="AH82" s="15"/>
+      <c r="AI82" s="19"/>
+      <c r="AJ82" s="19"/>
+      <c r="AK82" s="18"/>
+    </row>
+    <row r="83" spans="17:37" x14ac:dyDescent="0.25">
+      <c r="Q83" s="34"/>
+      <c r="S83" s="15"/>
+      <c r="T83" s="19"/>
+      <c r="U83" s="19"/>
+      <c r="V83" s="18"/>
+      <c r="W83" s="10"/>
+      <c r="X83" s="15"/>
+      <c r="Y83" s="19"/>
+      <c r="Z83" s="19"/>
+      <c r="AA83" s="18"/>
+      <c r="AB83" s="10"/>
+      <c r="AC83" s="15"/>
+      <c r="AD83" s="19"/>
+      <c r="AE83" s="19"/>
+      <c r="AF83" s="18"/>
+      <c r="AG83" s="10"/>
+      <c r="AH83" s="15"/>
+      <c r="AI83" s="19"/>
+      <c r="AJ83" s="19"/>
+      <c r="AK83" s="18"/>
+    </row>
+    <row r="84" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q84" s="35"/>
+      <c r="S84" s="23"/>
+      <c r="T84" s="25"/>
+      <c r="U84" s="25"/>
+      <c r="V84" s="26"/>
+      <c r="W84" s="10"/>
+      <c r="X84" s="23"/>
+      <c r="Y84" s="25"/>
+      <c r="Z84" s="25"/>
+      <c r="AA84" s="26"/>
+      <c r="AB84" s="10"/>
+      <c r="AC84" s="23"/>
+      <c r="AD84" s="25"/>
+      <c r="AE84" s="25"/>
+      <c r="AF84" s="26"/>
+      <c r="AG84" s="10"/>
+      <c r="AH84" s="23"/>
+      <c r="AI84" s="25"/>
+      <c r="AJ84" s="25"/>
+      <c r="AK84" s="26"/>
+    </row>
+    <row r="85" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="17:37" x14ac:dyDescent="0.25">
+      <c r="Q86" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="S86" s="3"/>
+      <c r="T86" s="8"/>
+      <c r="U86" s="5"/>
+      <c r="V86" s="6"/>
+      <c r="W86" s="31"/>
+      <c r="X86" s="7"/>
+      <c r="Y86" s="8"/>
+      <c r="Z86" s="8"/>
+      <c r="AA86" s="9"/>
+      <c r="AB86" s="31"/>
+      <c r="AC86" s="7"/>
+      <c r="AD86" s="8"/>
+      <c r="AE86" s="8"/>
+      <c r="AF86" s="9"/>
+      <c r="AG86" s="10"/>
+      <c r="AH86" s="7"/>
+      <c r="AI86" s="8"/>
+      <c r="AJ86" s="8"/>
+      <c r="AK86" s="9"/>
+    </row>
+    <row r="87" spans="17:37" x14ac:dyDescent="0.25">
+      <c r="Q87" s="34"/>
+      <c r="S87" s="11"/>
+      <c r="T87" s="12"/>
+      <c r="U87" s="13"/>
+      <c r="V87" s="14"/>
+      <c r="W87" s="31"/>
+      <c r="X87" s="15"/>
+      <c r="Y87" s="12"/>
+      <c r="Z87" s="12"/>
+      <c r="AA87" s="18"/>
+      <c r="AB87" s="31"/>
+      <c r="AC87" s="15"/>
+      <c r="AD87" s="12"/>
+      <c r="AE87" s="12"/>
+      <c r="AF87" s="18"/>
+      <c r="AG87" s="10"/>
+      <c r="AH87" s="15"/>
+      <c r="AI87" s="19"/>
+      <c r="AJ87" s="12"/>
+      <c r="AK87" s="18"/>
+    </row>
+    <row r="88" spans="17:37" x14ac:dyDescent="0.25">
+      <c r="Q88" s="34"/>
+      <c r="S88" s="11"/>
+      <c r="T88" s="12"/>
+      <c r="U88" s="12"/>
+      <c r="V88" s="18"/>
+      <c r="W88" s="31"/>
+      <c r="X88" s="15"/>
+      <c r="Y88" s="12"/>
+      <c r="Z88" s="19"/>
+      <c r="AA88" s="18"/>
+      <c r="AB88" s="31"/>
+      <c r="AC88" s="15"/>
+      <c r="AD88" s="19"/>
+      <c r="AE88" s="12"/>
+      <c r="AF88" s="18"/>
+      <c r="AG88" s="10"/>
+      <c r="AH88" s="15"/>
+      <c r="AI88" s="12"/>
+      <c r="AJ88" s="12"/>
+      <c r="AK88" s="18"/>
+    </row>
+    <row r="89" spans="17:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q89" s="35"/>
+      <c r="S89" s="20"/>
+      <c r="T89" s="21"/>
+      <c r="U89" s="21"/>
+      <c r="V89" s="22"/>
+      <c r="W89" s="31"/>
+      <c r="X89" s="23"/>
+      <c r="Y89" s="25"/>
+      <c r="Z89" s="25"/>
+      <c r="AA89" s="26"/>
+      <c r="AB89" s="31"/>
+      <c r="AC89" s="23"/>
+      <c r="AD89" s="25"/>
+      <c r="AE89" s="25"/>
+      <c r="AF89" s="26"/>
+      <c r="AG89" s="10"/>
+      <c r="AH89" s="23"/>
+      <c r="AI89" s="25"/>
+      <c r="AJ89" s="25"/>
+      <c r="AK89" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
+    <mergeCell ref="Q81:Q84"/>
+    <mergeCell ref="Q86:Q89"/>
+    <mergeCell ref="AR2:BJ2"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="Q66:Q74"/>
+    <mergeCell ref="Q76:Q79"/>
+    <mergeCell ref="Q46:Q54"/>
+    <mergeCell ref="Q56:Q59"/>
+    <mergeCell ref="Q16:Q24"/>
+    <mergeCell ref="Q36:Q39"/>
+    <mergeCell ref="Q41:Q44"/>
     <mergeCell ref="S4:V4"/>
     <mergeCell ref="X4:AA4"/>
     <mergeCell ref="AC4:AF4"/>
@@ -2365,18 +2566,6 @@
     <mergeCell ref="Q61:Q64"/>
     <mergeCell ref="Q26:Q34"/>
     <mergeCell ref="Q6:Q14"/>
-    <mergeCell ref="Q66:Q74"/>
-    <mergeCell ref="Q76:Q79"/>
-    <mergeCell ref="Q46:Q54"/>
-    <mergeCell ref="Q56:Q59"/>
-    <mergeCell ref="Q16:Q24"/>
-    <mergeCell ref="Q36:Q39"/>
-    <mergeCell ref="Q41:Q44"/>
-    <mergeCell ref="AR2:BJ2"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="AH2:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>